<commit_message>
nCCC, nUWE, etc added
</commit_message>
<xml_diff>
--- a/testData/studentsData.xlsx
+++ b/testData/studentsData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t xml:space="preserve">DeptYear</t>
   </si>
@@ -212,9 +212,6 @@
   </si>
   <si>
     <t xml:space="preserve">SOC4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UGG1</t>
   </si>
 </sst>
 </file>
@@ -325,7 +322,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B56" activeCellId="0" sqref="B56"/>
+      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="A64:B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -840,14 +837,6 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>